<commit_message>
[MOD] Modified ER model, changed images and tables for report
</commit_message>
<xml_diff>
--- a/values/operazioni.xlsx
+++ b/values/operazioni.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t xml:space="preserve">Operazione</t>
   </si>
@@ -28,28 +28,16 @@
     <t xml:space="preserve">Frequenza</t>
   </si>
   <si>
-    <t xml:space="preserve">Registrare un’associazione</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 ogni 10 anni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registrare un gruppo facente parte di un’associazione</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 ogni 10 giorni</t>
+    <t xml:space="preserve">Registrare un gruppo in un’associazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 ogni 5 anni</t>
   </si>
   <si>
     <t xml:space="preserve">Registrare un operatore e aggiungerlo ad un gruppo</t>
   </si>
   <si>
-    <t xml:space="preserve">5 ogni 10 giorni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizzare tutti i gruppi e membri di un’associazione</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registrare una casa produttrice</t>
+    <t xml:space="preserve">10 ogni 5 anni</t>
   </si>
   <si>
     <t xml:space="preserve">Registrare un ROV</t>
@@ -58,37 +46,43 @@
     <t xml:space="preserve">1 ogni 6 mesi</t>
   </si>
   <si>
-    <t xml:space="preserve">Registrare un manutentore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 ogni 3 anni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizzare tutti i dettagli di un ROV</t>
-  </si>
-  <si>
     <t xml:space="preserve">Registrare una spedizione</t>
   </si>
   <si>
-    <t xml:space="preserve">10 ogni 10 giorni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registrare un avvistamento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40 ogni 10 giorni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registrare un prelievo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 ogni 10 giorni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizzare gli avvistamenti con determinati filtri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.000 al giorno</t>
+    <t xml:space="preserve">1 ogni 2 giorni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registrare un avvistamento o prelievo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 ogni 2 giorni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare i dettagli di un ROV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 al mese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare gli avvistamenti con dei filtri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 al giorno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare il ROV usato in una spedizione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare gli operatori coinvolti in una spedizione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare gli operatori che hanno guidato un ROV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare le spedizioni avvenute in un luogo o paese</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare le analisi di un materiale</t>
   </si>
 </sst>
 </file>
@@ -104,6 +98,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -123,7 +118,7 @@
     <font>
       <b val="true"/>
       <sz val="20"/>
-      <color rgb="FFFAFAFA"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -132,6 +127,7 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -143,8 +139,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF536DFE"/>
-        <bgColor rgb="FF666699"/>
+        <fgColor rgb="FF00CDFF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -157,8 +153,8 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
+      <left style="thin"/>
+      <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
@@ -194,20 +190,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -222,7 +218,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFAFAFA"/>
+      <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -253,7 +249,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FF00CDFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
@@ -261,7 +257,7 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF536DFE"/>
+      <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
@@ -283,35 +279,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="66.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="66.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -324,10 +320,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -336,72 +332,76 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>3</v>
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>16</v>
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>20</v>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
[FIX] Fixed ER model and tables
</commit_message>
<xml_diff>
--- a/values/operazioni.xlsx
+++ b/values/operazioni.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+  <si>
+    <t xml:space="preserve">Codice</t>
+  </si>
   <si>
     <t xml:space="preserve">Operazione</t>
   </si>
@@ -28,67 +31,117 @@
     <t xml:space="preserve">Frequenza</t>
   </si>
   <si>
-    <t xml:space="preserve">Registrare un operatore e aggiungerlo ad un gruppo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 ogni 5 anni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registrare un ROV</t>
+    <t xml:space="preserve">O1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggiungere un operatore ad un gruppo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 ogni 3 anni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registrare un nuovo ROV</t>
   </si>
   <si>
     <t xml:space="preserve">1 ogni 6 mesi</t>
   </si>
   <si>
+    <t xml:space="preserve">O3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Registrare una spedizione</t>
   </si>
   <si>
-    <t xml:space="preserve">1 ogni 2 giorni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registrare un avvistamento o prelievo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 ogni 2 giorni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizzare i dettagli di un ROV</t>
+    <t xml:space="preserve">1 ogni 2 mesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggiungere un avvistamento o prelievo in una spedizione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 ogni 2 mesi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificare la specie di un organismo e rimuovere il nome provvisorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 ogni 4 anni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare avvistamenti e prelievi con dei filtri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 al giorno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare le spedizioni organizzate da un’associazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 all’anno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare i dettagli di una spedizione (luogo, ROV utilizzato, gruppo e operatori che hanno partecipato)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 al giorno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare gli organismi avvistati in una  spedizione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare le formazioni geologiche di un determinato grado di pericolo e dove sono situate</t>
   </si>
   <si>
     <t xml:space="preserve">1 al mese</t>
   </si>
   <si>
-    <t xml:space="preserve">Visualizzare gli avvistamenti e i prelievi con dei filtri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 al giorno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizzare il ROV usato in una spedizione</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizzare le spedizioni avvenute in un luogo o paese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizzare le analisi di un materiale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizzare l’associazione che ha organizzato una spedizione e il gruppo e gli operatori che hanno partecipato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizzare le spedizioni organizzate da un’associazione</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 all’anno</t>
+    <t xml:space="preserve">O11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare i luoghi dove sono affondati determinati relitti (sapendo il nome)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare le descrizioni e le foto degli incontri con un organismo e i luoghi dove è stato avvistato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare le analisi fatte su un determinato materiale e i laboratori che le hanno effettuate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -114,14 +167,13 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
+      <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -136,8 +188,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00CDFF"/>
-        <bgColor rgb="FF33CCCC"/>
+        <fgColor rgb="FF40C4FF"/>
+        <bgColor rgb="FF00CCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -182,24 +234,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -246,7 +294,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CDFF"/>
+      <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
@@ -255,7 +303,7 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF40C4FF"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -280,112 +328,171 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="66.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.97"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="23.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="51.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="21.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[MOD] Modified some attributes
</commit_message>
<xml_diff>
--- a/values/operazioni.xlsx
+++ b/values/operazioni.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t xml:space="preserve">Codice</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Registrare una spedizione</t>
   </si>
   <si>
-    <t xml:space="preserve">1 ogni 2 settimane</t>
+    <t xml:space="preserve">1 ogni 10 giorni</t>
   </si>
   <si>
     <t xml:space="preserve">O4</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Aggiungere un avvistamento o prelievo in una spedizione</t>
   </si>
   <si>
-    <t xml:space="preserve">10 ogni 2 settimane</t>
+    <t xml:space="preserve">10 ogni 10 giorni</t>
   </si>
   <si>
     <t xml:space="preserve">O5</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">O9</t>
   </si>
   <si>
-    <t xml:space="preserve">Visualizzare le formazioni geologiche di un determinato grado di pericolo e dove sono situate</t>
+    <t xml:space="preserve">Visualizzare i luoghi più pericolosi</t>
   </si>
   <si>
     <t xml:space="preserve">1 al mese</t>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t xml:space="preserve">Visualizzare le analisi fatte su un materiale e da quale laboratorio sono state eseguite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizzare quanti organismi vengono scoperti ogni anno</t>
   </si>
 </sst>
 </file>
@@ -313,13 +319,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51"/>
@@ -425,7 +431,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
@@ -456,6 +462,17 @@
       </c>
       <c r="C12" s="3" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>